<commit_message>
added CMCSA and others
</commit_message>
<xml_diff>
--- a/SAVA.xlsx
+++ b/SAVA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinshkreli/code/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BDF85B-E66A-4427-A938-5AF1CE06118C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7359B9C-E3BC-754A-BBB8-65D35A494C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51720" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{E72B2B4C-5C13-AF4D-850F-73D2746B3A7A}"/>
+    <workbookView xWindow="-39740" yWindow="-20760" windowWidth="32720" windowHeight="16660" activeTab="1" xr2:uid="{E72B2B4C-5C13-AF4D-850F-73D2746B3A7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -658,7 +658,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -737,15 +737,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -855,7 +846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -900,11 +891,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1407,20 +1396,20 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
-    <col min="4" max="8" width="10.875" style="1"/>
-    <col min="9" max="9" width="7.375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.75" style="1" customWidth="1"/>
-    <col min="12" max="12" width="2.625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.875" style="1"/>
+    <col min="4" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="7.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B2" s="16" t="s">
         <v>7</v>
       </c>
@@ -1438,7 +1427,7 @@
         <v>28.75</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
@@ -1456,7 +1445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B4" s="12"/>
       <c r="G4" s="11"/>
       <c r="I4" s="1" t="s">
@@ -1467,7 +1456,7 @@
         <v>1379.3147724999999</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B5" s="12"/>
       <c r="G5" s="11"/>
       <c r="I5" s="1" t="s">
@@ -1480,7 +1469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B6" s="12"/>
       <c r="G6" s="11"/>
       <c r="I6" s="1" t="s">
@@ -1493,7 +1482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B7" s="12"/>
       <c r="G7" s="11"/>
       <c r="I7" s="1" t="s">
@@ -1504,7 +1493,7 @@
         <v>1172.0237725</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -1516,15 +1505,15 @@
         <v>4.3207079115075597</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.15">
       <c r="J9" s="27"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.15">
       <c r="I10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.15">
       <c r="H17" s="27"/>
     </row>
   </sheetData>
@@ -1539,97 +1528,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95ABFF95-7EFA-4FFF-9E22-334733664B4D}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.83203125" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B2" s="34" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B3" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B4" s="34" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B6" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="34" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B7" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="34" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="38" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B10" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B11" s="34" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B12" s="34" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B13" s="34" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="38" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B15" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B16" s="34" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B17" s="34" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B18" s="34" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B19" s="34" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Main!A1" display="Main" xr:uid="{281B8411-A076-8846-AFAE-894534B26E9A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1640,21 +1633,21 @@
   <sheetViews>
     <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" style="1" customWidth="1"/>
-    <col min="3" max="6" width="10.875" style="1"/>
-    <col min="7" max="7" width="16.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1662,7 +1655,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1670,7 +1663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1682,7 +1675,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1699,7 +1692,7 @@
         <v>2100000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B8" s="8" t="s">
         <v>22</v>
       </c>
@@ -1710,7 +1703,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1721,7 +1714,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1738,7 +1731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1749,7 +1742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C12" s="2"/>
       <c r="D12" s="9"/>
       <c r="E12" s="30" t="s">
@@ -1759,7 +1752,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B13" s="27" t="s">
         <v>148</v>
       </c>
@@ -1778,7 +1771,7 @@
         <v>0.81818181818181812</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B14" s="27" t="s">
         <v>150</v>
       </c>
@@ -1797,7 +1790,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B15" s="27" t="s">
         <v>149</v>
       </c>
@@ -1816,7 +1809,7 @@
         <v>1.3333333333333335</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B17" s="27" t="s">
         <v>155</v>
       </c>
@@ -1835,7 +1828,7 @@
         <v>-2.8181818181818183</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B18" s="27" t="s">
         <v>154</v>
       </c>
@@ -1854,7 +1847,7 @@
         <v>0.81818181818181812</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B19" s="27" t="s">
         <v>156</v>
       </c>
@@ -1887,19 +1880,19 @@
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.875" style="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1907,7 +1900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1915,7 +1908,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1923,7 +1916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1931,7 +1924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" s="22" t="s">
         <v>75</v>
       </c>
@@ -1939,7 +1932,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B7" s="22"/>
       <c r="C7" s="23">
         <f>1100*0.5^6*0.6</f>
@@ -1953,7 +1946,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B8" s="20" t="s">
         <v>46</v>
       </c>
@@ -1961,62 +1954,62 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C14" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C15" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C18" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C22" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C23" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C24" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.15">
       <c r="D26" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.15">
       <c r="D27" s="6" t="s">
         <v>40</v>
       </c>
@@ -2024,13 +2017,13 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.15">
       <c r="D28" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C29" s="35" t="s">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="C29" s="34" t="s">
         <v>191</v>
       </c>
       <c r="D29" s="21">
@@ -2040,17 +2033,17 @@
         <f>D29-0.9</f>
         <v>18.400000000000002</v>
       </c>
-      <c r="F29" s="37">
+      <c r="F29" s="36">
         <f>E29/D29-1</f>
         <v>-4.663212435233155E-2</v>
       </c>
-      <c r="G29" s="36">
+      <c r="G29" s="35">
         <f>+D29-E29</f>
         <v>0.89999999999999858</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C30" s="35" t="s">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="C30" s="34" t="s">
         <v>192</v>
       </c>
       <c r="D30" s="21">
@@ -2060,142 +2053,142 @@
         <f>D30-1.5</f>
         <v>20.399999999999999</v>
       </c>
-      <c r="F30" s="37">
+      <c r="F30" s="36">
         <f>E30/D30-1</f>
         <v>-6.8493150684931559E-2</v>
       </c>
-      <c r="G30" s="36">
+      <c r="G30" s="35">
         <f>+D30-E30</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.15">
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C32" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C34" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C35" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C36" s="22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.15">
       <c r="H39" s="22"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C40" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C41" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C42" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.15">
       <c r="C43" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C90" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C91" s="20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C93" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C94" s="20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C97" s="20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C101" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C102" s="20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C103" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C106" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C111" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C112" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C113" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C114" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C115" s="22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C116" s="22" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C120" s="24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C121" s="24" t="s">
         <v>89</v>
       </c>
@@ -2215,158 +2208,158 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>183</v>
       </c>
@@ -2387,22 +2380,22 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.875" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="45.875" style="25" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" style="25" customWidth="1"/>
     <col min="4" max="4" width="9" style="25"/>
-    <col min="5" max="5" width="10.25" style="25" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" style="25" customWidth="1"/>
     <col min="6" max="16384" width="9" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="25" t="s">
         <v>90</v>
@@ -2411,7 +2404,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="25" t="s">
         <v>92</v>
@@ -2420,7 +2413,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="25" t="s">
         <v>94</v>
@@ -2429,7 +2422,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="25" t="s">
         <v>96</v>
@@ -2438,25 +2431,25 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="5"/>
       <c r="C6" s="25" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="5"/>
       <c r="C7" s="25" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="5"/>
       <c r="C8" s="25" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="5"/>
       <c r="B9" s="25" t="s">
         <v>99</v>
@@ -2465,25 +2458,25 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="5"/>
       <c r="C10" s="25" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="5"/>
       <c r="C11" s="25" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="5"/>
       <c r="C12" s="25" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="5"/>
       <c r="B13" s="25" t="s">
         <v>135</v>
@@ -2492,7 +2485,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="5"/>
       <c r="B14" s="25" t="s">
         <v>103</v>
@@ -2501,13 +2494,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="5"/>
       <c r="C15" s="25" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="5"/>
       <c r="B16" s="25" t="s">
         <v>122</v>
@@ -2516,7 +2509,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="5"/>
       <c r="B17" s="25" t="s">
         <v>106</v>
@@ -2525,7 +2518,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="5"/>
       <c r="B18" s="25" t="s">
         <v>108</v>
@@ -2534,7 +2527,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="5"/>
       <c r="B19" s="25" t="s">
         <v>110</v>
@@ -2543,15 +2536,15 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B21" s="25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B22" s="25" t="s">
         <v>58</v>
       </c>
@@ -2559,7 +2552,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B23" s="25" t="s">
         <v>60</v>
       </c>
@@ -2567,7 +2560,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B24" s="25" t="s">
         <v>62</v>
       </c>
@@ -2575,7 +2568,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B25" s="25" t="s">
         <v>65</v>
       </c>
@@ -2583,7 +2576,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B26" s="25" t="s">
         <v>66</v>
       </c>
@@ -2591,7 +2584,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B27" s="25" t="s">
         <v>69</v>
       </c>
@@ -2599,7 +2592,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B28" s="25" t="s">
         <v>71</v>
       </c>
@@ -2607,7 +2600,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B29" s="25" t="s">
         <v>73</v>
       </c>
@@ -2615,17 +2608,17 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="F30" s="25" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B32" s="25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B34" s="25" t="s">
         <v>114</v>
       </c>
@@ -2633,132 +2626,132 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C35" s="25" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C36" s="25" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C37" s="25" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C38" s="25" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C39" s="25" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C40" s="25" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C41" s="25" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C42" s="25" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C43" s="25" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C44" s="25" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C45" s="25" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C47" s="26" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C48" s="25" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C49" s="25" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C50" s="25" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C51" s="25" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C52" s="25" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C53" s="25" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C54" s="25" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C55" s="25" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C56" s="25" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C57" s="25" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C58" s="25" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C59" s="25" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C60" s="25" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C61" s="25" t="s">
         <v>147</v>
       </c>
@@ -2780,24 +2773,24 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>85</v>
       </c>

</xml_diff>